<commit_message>
creation class et methode
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26220"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3EB8000A-B787-455E-80DA-1D4F78A5D0E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6BB3FBA-6D9F-4A4C-A7DE-00F450F19DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Actions #</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Action-12</t>
   </si>
   <si>
-    <t> 9%</t>
-  </si>
-  <si>
     <t>Action-13</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
   </si>
   <si>
     <t>Action-19</t>
-  </si>
-  <si>
-    <t>24 </t>
   </si>
   <si>
     <t>Action-20</t>
@@ -148,8 +142,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,24 +460,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -494,7 +488,7 @@
       <c r="B2">
         <v>20</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>0.05</v>
       </c>
     </row>
@@ -505,7 +499,7 @@
       <c r="B3">
         <v>30</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>0.1</v>
       </c>
     </row>
@@ -516,7 +510,7 @@
       <c r="B4">
         <v>50</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
         <v>0.15</v>
       </c>
     </row>
@@ -527,7 +521,7 @@
       <c r="B5">
         <v>70</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2">
         <v>0.2</v>
       </c>
     </row>
@@ -538,7 +532,7 @@
       <c r="B6">
         <v>60</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2">
         <v>0.17</v>
       </c>
     </row>
@@ -549,7 +543,7 @@
       <c r="B7">
         <v>80</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="2">
         <v>0.25</v>
       </c>
     </row>
@@ -560,7 +554,7 @@
       <c r="B8">
         <v>22</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
@@ -571,7 +565,7 @@
       <c r="B9">
         <v>26</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>0.11</v>
       </c>
     </row>
@@ -582,7 +576,7 @@
       <c r="B10">
         <v>48</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <v>0.13</v>
       </c>
     </row>
@@ -593,7 +587,7 @@
       <c r="B11">
         <v>34</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <v>0.27</v>
       </c>
     </row>
@@ -604,7 +598,7 @@
       <c r="B12">
         <v>42</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="2">
         <v>0.17</v>
       </c>
     </row>
@@ -615,95 +609,95 @@
       <c r="B13">
         <v>110</v>
       </c>
-      <c r="C13" t="s">
-        <v>15</v>
+      <c r="C13" s="2">
+        <v>0.09</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>38</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="2">
         <v>0.23</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="2">
         <v>0.01</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>18</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="2">
         <v>0.03</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>8</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="2">
         <v>0.08</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>4</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="2">
         <v>0.12</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>10</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="2">
         <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="1">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>24</v>
+      </c>
+      <c r="C20" s="2">
         <v>0.21</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>114</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="2">
         <v>0.18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modifications mais resultat toujours different. A verif : pb int vs float dans les conversions
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26220"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26301"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6BB3FBA-6D9F-4A4C-A7DE-00F450F19DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8AC2A3A5-88C9-45CB-8AB2-330858F50597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -140,10 +140,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,14 +459,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -488,8 +487,8 @@
       <c r="B2">
         <v>20</v>
       </c>
-      <c r="C2" s="2">
-        <v>0.05</v>
+      <c r="C2">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -499,8 +498,8 @@
       <c r="B3">
         <v>30</v>
       </c>
-      <c r="C3" s="2">
-        <v>0.1</v>
+      <c r="C3">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -510,8 +509,8 @@
       <c r="B4">
         <v>50</v>
       </c>
-      <c r="C4" s="2">
-        <v>0.15</v>
+      <c r="C4">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -521,8 +520,8 @@
       <c r="B5">
         <v>70</v>
       </c>
-      <c r="C5" s="2">
-        <v>0.2</v>
+      <c r="C5">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -532,8 +531,8 @@
       <c r="B6">
         <v>60</v>
       </c>
-      <c r="C6" s="2">
-        <v>0.17</v>
+      <c r="C6">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -543,8 +542,8 @@
       <c r="B7">
         <v>80</v>
       </c>
-      <c r="C7" s="2">
-        <v>0.25</v>
+      <c r="C7">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -554,8 +553,8 @@
       <c r="B8">
         <v>22</v>
       </c>
-      <c r="C8" s="2">
-        <v>7.0000000000000007E-2</v>
+      <c r="C8">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -565,8 +564,8 @@
       <c r="B9">
         <v>26</v>
       </c>
-      <c r="C9" s="2">
-        <v>0.11</v>
+      <c r="C9">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -576,8 +575,8 @@
       <c r="B10">
         <v>48</v>
       </c>
-      <c r="C10" s="2">
-        <v>0.13</v>
+      <c r="C10">
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -587,8 +586,8 @@
       <c r="B11">
         <v>34</v>
       </c>
-      <c r="C11" s="2">
-        <v>0.27</v>
+      <c r="C11">
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -598,8 +597,8 @@
       <c r="B12">
         <v>42</v>
       </c>
-      <c r="C12" s="2">
-        <v>0.17</v>
+      <c r="C12">
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -609,8 +608,8 @@
       <c r="B13">
         <v>110</v>
       </c>
-      <c r="C13" s="2">
-        <v>0.09</v>
+      <c r="C13">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -620,8 +619,8 @@
       <c r="B14">
         <v>38</v>
       </c>
-      <c r="C14" s="2">
-        <v>0.23</v>
+      <c r="C14">
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -631,8 +630,8 @@
       <c r="B15">
         <v>14</v>
       </c>
-      <c r="C15" s="2">
-        <v>0.01</v>
+      <c r="C15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -642,8 +641,8 @@
       <c r="B16">
         <v>18</v>
       </c>
-      <c r="C16" s="2">
-        <v>0.03</v>
+      <c r="C16">
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -653,8 +652,8 @@
       <c r="B17">
         <v>8</v>
       </c>
-      <c r="C17" s="2">
-        <v>0.08</v>
+      <c r="C17">
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -664,8 +663,8 @@
       <c r="B18">
         <v>4</v>
       </c>
-      <c r="C18" s="2">
-        <v>0.12</v>
+      <c r="C18">
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -675,8 +674,8 @@
       <c r="B19">
         <v>10</v>
       </c>
-      <c r="C19" s="2">
-        <v>0.14000000000000001</v>
+      <c r="C19">
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -686,8 +685,8 @@
       <c r="B20">
         <v>24</v>
       </c>
-      <c r="C20" s="2">
-        <v>0.21</v>
+      <c r="C20">
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -697,8 +696,8 @@
       <c r="B21">
         <v>114</v>
       </c>
-      <c r="C21" s="2">
-        <v>0.18</v>
+      <c r="C21">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>